<commit_message>
making changes to data for presentation example
</commit_message>
<xml_diff>
--- a/inst/presentations/using-dragondown/live-examples/data/Elrod_2020_2_17_Treated_Virgin.xlsx
+++ b/inst/presentations/using-dragondown/live-examples/data/Elrod_2020_2_17_Treated_Virgin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asajc\OneDrive - Drexel University\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\R\Projects\dragondown\inst\presentations\using-dragondown\live-examples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="644" documentId="8_{4FF06616-7D5D-4037-BDC2-7163DDD96BF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BF645A15-AFBF-470A-979C-4E51B11F9B12}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C22A68-B428-40AF-A406-291D0D0F687C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{4C9902C0-AEC6-4530-A0F5-E9DE864CF67A}"/>
+    <workbookView xWindow="20250" yWindow="2685" windowWidth="31200" windowHeight="17760" xr2:uid="{4C9902C0-AEC6-4530-A0F5-E9DE864CF67A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -656,18 +654,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DFC4C6-6C8B-4A36-A6E6-F190DFCEF772}">
   <dimension ref="A4:B273"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -675,7 +674,7 @@
         <v>399.19828716199999</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -683,7 +682,7 @@
         <v>368.68503992400002</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -691,7 +690,7 @@
         <v>383.74664108600001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -699,15 +698,15 @@
         <v>420.48191453700002</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8">
-        <v>400.50818205600001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <v>410.50818205600001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -715,7 +714,7 @@
         <v>409.21217335900002</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -723,7 +722,7 @@
         <v>310.265194522</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -731,7 +730,7 @@
         <v>324.61174729700002</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -739,7 +738,7 @@
         <v>317.53277335900003</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -747,7 +746,7 @@
         <v>374.285377939</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -755,7 +754,7 @@
         <v>354.348673749</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -763,7 +762,7 @@
         <v>368.46730134900002</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -771,7 +770,7 @@
         <v>416.650377746</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -779,7 +778,7 @@
         <v>404.12040134900002</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -787,7 +786,7 @@
         <v>402.03627392200002</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -795,7 +794,7 @@
         <v>305.883275733</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -803,7 +802,7 @@
         <v>326.14462686500002</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -811,7 +810,7 @@
         <v>317.54499727900003</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -819,7 +818,7 @@
         <v>404.07649710300001</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -827,7 +826,7 @@
         <v>385.52980541599999</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -835,7 +834,7 @@
         <v>399.03632022200003</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -843,15 +842,15 @@
         <v>381.70341285800004</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
       <c r="B26">
-        <v>377.43100001900001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+        <v>397.43100001900001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -859,7 +858,7 @@
         <v>400.14706708599999</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -867,7 +866,7 @@
         <v>345.95567934400003</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -875,7 +874,7 @@
         <v>346.46862558700002</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -883,7 +882,7 @@
         <v>343.97255205599998</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -891,7 +890,7 @@
         <v>417.84964616400003</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -899,7 +898,7 @@
         <v>397.45235485500001</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -907,7 +906,7 @@
         <v>406.62121164900003</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -915,7 +914,7 @@
         <v>353.07035731500002</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -923,7 +922,7 @@
         <v>333.19074901800002</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -931,7 +930,7 @@
         <v>343.00075041600002</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -939,7 +938,7 @@
         <v>434.74111721700001</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -947,7 +946,7 @@
         <v>405.09230485500001</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -955,7 +954,7 @@
         <v>409.21365041600001</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -963,7 +962,7 @@
         <v>345.99688414100001</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -971,7 +970,7 @@
         <v>324.734292095</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -979,7 +978,7 @@
         <v>332.81267335900003</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -987,7 +986,7 @@
         <v>427.43167145400002</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -995,7 +994,7 @@
         <v>419.81744261900002</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -1003,7 +1002,7 @@
         <v>422.40952485500003</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -1011,7 +1010,7 @@
         <v>426.165629873</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -1019,7 +1018,7 @@
         <v>423.12472604100003</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -1027,7 +1026,7 @@
         <v>424.49304108600001</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -1035,7 +1034,7 @@
         <v>289.29210564800002</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -1043,7 +1042,7 @@
         <v>268.85478100099999</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -1051,7 +1050,7 @@
         <v>276.78785041600003</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -1059,7 +1058,7 @@
         <v>267.18896630300003</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -1067,7 +1066,7 @@
         <v>256.40599180600003</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -1075,7 +1074,7 @@
         <v>260.95176205600001</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -1083,7 +1082,7 @@
         <v>294.99186487899999</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>17</v>
       </c>
@@ -1091,7 +1090,7 @@
         <v>286.45386422299998</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>289.98372485499999</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -1107,7 +1106,7 @@
         <v>203.697569292</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -1115,15 +1114,15 @@
         <v>222.886475176</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>18</v>
       </c>
       <c r="B60">
-        <v>205.48017335900002</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+        <v>215.48017335899999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -1131,7 +1130,7 @@
         <v>290.73172689300003</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -1139,7 +1138,7 @@
         <v>263.50116243799999</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -1147,7 +1146,7 @@
         <v>266.60634371600003</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -1155,7 +1154,7 @@
         <v>210.73116192700002</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -1163,7 +1162,7 @@
         <v>238.256373787</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>20</v>
       </c>
@@ -1171,7 +1170,7 @@
         <v>221.733352056</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>21</v>
       </c>
@@ -1179,7 +1178,7 @@
         <v>294.61771106100002</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>21</v>
       </c>
@@ -1187,7 +1186,7 @@
         <v>271.82458236500003</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>21</v>
       </c>
@@ -1195,7 +1194,7 @@
         <v>281.87967335900004</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>22</v>
       </c>
@@ -1203,7 +1202,7 @@
         <v>297.62184126700004</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>22</v>
       </c>
@@ -1211,7 +1210,7 @@
         <v>281.49828705499999</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>22</v>
       </c>
@@ -1219,7 +1218,7 @@
         <v>286.97445041600002</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>23</v>
       </c>
@@ -1227,7 +1226,7 @@
         <v>297.95438282399999</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>23</v>
       </c>
@@ -1235,7 +1234,7 @@
         <v>292.07671462400003</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>23</v>
       </c>
@@ -1243,7 +1242,7 @@
         <v>294.054137416</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>24</v>
       </c>
@@ -1251,7 +1250,7 @@
         <v>216.811645333</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>24</v>
       </c>
@@ -1259,7 +1258,7 @@
         <v>209.918220314</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>24</v>
       </c>
@@ -1267,7 +1266,7 @@
         <v>214.094420716</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>25</v>
       </c>
@@ -1275,7 +1274,7 @@
         <v>296.827184601</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>25</v>
       </c>
@@ -1283,7 +1282,7 @@
         <v>290.35563762100003</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>25</v>
       </c>
@@ -1291,7 +1290,7 @@
         <v>293.03955205599999</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>26</v>
       </c>
@@ -1299,7 +1298,7 @@
         <v>299.43490326800003</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>26</v>
       </c>
@@ -1307,7 +1306,7 @@
         <v>275.53082397600002</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>26</v>
       </c>
@@ -1315,7 +1314,7 @@
         <v>289.98357205600001</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>27</v>
       </c>
@@ -1323,7 +1322,7 @@
         <v>282.18720681299999</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>27</v>
       </c>
@@ -1331,7 +1330,7 @@
         <v>251.371825019</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>27</v>
       </c>
@@ -1339,7 +1338,7 @@
         <v>260.95176205600001</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>28</v>
       </c>
@@ -1347,7 +1346,7 @@
         <v>252.10266263600002</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>28</v>
       </c>
@@ -1355,7 +1354,7 @@
         <v>222.797087761</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>28</v>
       </c>
@@ -1363,7 +1362,7 @@
         <v>236.040941086</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>29</v>
       </c>
@@ -1371,7 +1370,7 @@
         <v>286.84273767799999</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>29</v>
       </c>
@@ -1379,7 +1378,7 @@
         <v>251.82217460500001</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>29</v>
       </c>
@@ -1387,7 +1386,7 @@
         <v>266.59977335899998</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>30</v>
       </c>
@@ -1395,7 +1394,7 @@
         <v>121.872889864</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>30</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>112.826017605</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>30</v>
       </c>
@@ -1411,7 +1410,7 @@
         <v>112.222869019</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>31</v>
       </c>
@@ -1419,7 +1418,7 @@
         <v>104.658197993</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>31</v>
       </c>
@@ -1427,7 +1426,7 @@
         <v>101.180696485</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>31</v>
       </c>
@@ -1435,7 +1434,7 @@
         <v>103.003945086</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>32</v>
       </c>
@@ -1443,7 +1442,7 @@
         <v>125.677126567</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>32</v>
       </c>
@@ -1451,7 +1450,7 @@
         <v>120.13184712500001</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>32</v>
       </c>
@@ -1459,7 +1458,7 @@
         <v>119.867352056</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>33</v>
       </c>
@@ -1467,7 +1466,7 @@
         <v>82.723901542999997</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>33</v>
       </c>
@@ -1475,7 +1474,7 @@
         <v>91.10696401300001</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>33</v>
       </c>
@@ -1483,7 +1482,7 @@
         <v>89.307552056000006</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>34</v>
       </c>
@@ -1491,7 +1490,7 @@
         <v>125.424651686</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>34</v>
       </c>
@@ -1499,7 +1498,7 @@
         <v>122.664388684</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>34</v>
       </c>
@@ -1507,7 +1506,7 @@
         <v>123.931907322</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>35</v>
       </c>
@@ -1515,7 +1514,7 @@
         <v>114.863286672</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>35</v>
       </c>
@@ -1523,7 +1522,7 @@
         <v>103.059003659</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>35</v>
       </c>
@@ -1531,7 +1530,7 @@
         <v>99.274834558000009</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>36</v>
       </c>
@@ -1539,7 +1538,7 @@
         <v>125.985016552</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>36</v>
       </c>
@@ -1547,7 +1546,7 @@
         <v>122.41415485500001</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>36</v>
       </c>
@@ -1555,7 +1554,7 @@
         <v>118.72176702</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>37</v>
       </c>
@@ -1563,7 +1562,7 @@
         <v>116.74526102200001</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>37</v>
       </c>
@@ -1571,7 +1570,7 @@
         <v>110.14271436600001</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>37</v>
       </c>
@@ -1579,7 +1578,7 @@
         <v>113.602593056</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>38</v>
       </c>
@@ -1587,7 +1586,7 @@
         <v>121.632689836</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>38</v>
       </c>
@@ -1595,7 +1594,7 @@
         <v>119.45846193200001</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>38</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>120.37668205600001</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>39</v>
       </c>
@@ -1611,7 +1610,7 @@
         <v>123.14967830800001</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>39</v>
       </c>
@@ -1619,7 +1618,7 @@
         <v>120.88453499900001</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>39</v>
       </c>
@@ -1627,7 +1626,7 @@
         <v>122.414002056</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>40</v>
       </c>
@@ -1635,7 +1634,7 @@
         <v>110.154989219</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>40</v>
       </c>
@@ -1643,7 +1642,7 @@
         <v>111.20874205600001</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>40</v>
       </c>
@@ -1651,7 +1650,7 @@
         <v>112.291526703</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>41</v>
       </c>
@@ -1659,7 +1658,7 @@
         <v>119.69000335</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>41</v>
       </c>
@@ -1667,7 +1666,7 @@
         <v>117.320702056</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>41</v>
       </c>
@@ -1675,7 +1674,7 @@
         <v>112.789294912</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>42</v>
       </c>
@@ -1683,7 +1682,7 @@
         <v>122.174260425</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>42</v>
       </c>
@@ -1691,7 +1690,7 @@
         <v>113.209339363</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>42</v>
       </c>
@@ -1699,7 +1698,7 @@
         <v>117.320702056</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>43</v>
       </c>
@@ -1707,7 +1706,7 @@
         <v>122.77068585500001</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>43</v>
       </c>
@@ -1715,7 +1714,7 @@
         <v>124.94257084100001</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>43</v>
       </c>
@@ -1723,7 +1722,7 @@
         <v>125.46998205600001</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>44</v>
       </c>
@@ -1731,7 +1730,7 @@
         <v>121.726610288</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>44</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>111.27841840000001</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>44</v>
       </c>
@@ -1747,7 +1746,7 @@
         <v>114.26574071600001</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>45</v>
       </c>
@@ -1755,7 +1754,7 @@
         <v>294.55389201200001</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>45</v>
       </c>
@@ -1763,7 +1762,7 @@
         <v>337.61560432600004</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>45</v>
       </c>
@@ -1771,7 +1770,7 @@
         <v>307.34765041600002</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>46</v>
       </c>
@@ -1779,7 +1778,7 @@
         <v>380.195592326</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>46</v>
       </c>
@@ -1787,7 +1786,7 @@
         <v>408.32257758100002</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>46</v>
       </c>
@@ -1795,7 +1794,7 @@
         <v>393.93375041600001</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>47</v>
       </c>
@@ -1803,7 +1802,7 @@
         <v>337.30221357700003</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>47</v>
       </c>
@@ -1811,7 +1810,7 @@
         <v>333.78610485500002</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>47</v>
       </c>
@@ -1819,7 +1818,7 @@
         <v>323.81133520200001</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>48</v>
       </c>
@@ -1827,7 +1826,7 @@
         <v>92.106982535</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>48</v>
       </c>
@@ -1835,7 +1834,7 @@
         <v>88.679293501000004</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>48</v>
       </c>
@@ -1843,7 +1842,7 @@
         <v>90.326364855000008</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>49</v>
       </c>
@@ -1851,7 +1850,7 @@
         <v>108.033833501</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>49</v>
       </c>
@@ -1859,7 +1858,7 @@
         <v>98.102102232999997</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>49</v>
       </c>
@@ -1867,7 +1866,7 @@
         <v>102.041820716</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>50</v>
       </c>
@@ -1875,7 +1874,7 @@
         <v>87.432657393</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>50</v>
       </c>
@@ -1883,7 +1882,7 @@
         <v>83.240922425999997</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>50</v>
       </c>
@@ -1891,7 +1890,7 @@
         <v>75.245409152999997</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>51</v>
       </c>
@@ -1899,7 +1898,7 @@
         <v>49.327337175000004</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>51</v>
       </c>
@@ -1907,7 +1906,7 @@
         <v>49.555415149000005</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>51</v>
       </c>
@@ -1915,7 +1914,7 @@
         <v>49.422581885</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>52</v>
       </c>
@@ -1923,7 +1922,7 @@
         <v>50.277950687000001</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>52</v>
       </c>
@@ -1931,7 +1930,7 @@
         <v>51.107802056000004</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>52</v>
       </c>
@@ -1939,7 +1938,7 @@
         <v>52.545640646000003</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>53</v>
       </c>
@@ -1947,7 +1946,7 @@
         <v>47.450201460000002</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>53</v>
       </c>
@@ -1955,7 +1954,7 @@
         <v>49.269681019000004</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>53</v>
       </c>
@@ -1963,7 +1962,7 @@
         <v>51.674533547000003</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>54</v>
       </c>
@@ -1971,7 +1970,7 @@
         <v>48.785511921000001</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>54</v>
       </c>
@@ -1979,7 +1978,7 @@
         <v>44.087197336000003</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>54</v>
       </c>
@@ -1987,7 +1986,7 @@
         <v>45.500588086</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>55</v>
       </c>
@@ -1995,7 +1994,7 @@
         <v>56.474153868999998</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>55</v>
       </c>
@@ -2003,7 +2002,7 @@
         <v>55.509839380000003</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>55</v>
       </c>
@@ -2011,7 +2010,7 @@
         <v>55.636306019000003</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>56</v>
       </c>
@@ -2019,7 +2018,7 @@
         <v>42.737218171000002</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>56</v>
       </c>
@@ -2027,7 +2026,7 @@
         <v>45.347840019000003</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>56</v>
       </c>
@@ -2035,7 +2034,7 @@
         <v>48.149256885</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>57</v>
       </c>
@@ -2043,7 +2042,7 @@
         <v>52.760068576000002</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>57</v>
       </c>
@@ -2051,7 +2050,7 @@
         <v>50.846464832999999</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>57</v>
       </c>
@@ -2059,7 +2058,7 @@
         <v>51.107954855000003</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>58</v>
       </c>
@@ -2067,7 +2066,7 @@
         <v>61.452701820000001</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>58</v>
       </c>
@@ -2075,7 +2074,7 @@
         <v>59.766564854999999</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>58</v>
       </c>
@@ -2083,7 +2082,7 @@
         <v>58.924897030000004</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>59</v>
       </c>
@@ -2091,7 +2090,7 @@
         <v>61.085016493000005</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>59</v>
       </c>
@@ -2099,7 +2098,7 @@
         <v>60.785224855000003</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>59</v>
       </c>
@@ -2107,7 +2106,7 @@
         <v>59.714715061</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>60</v>
       </c>
@@ -2115,7 +2114,7 @@
         <v>229.56180508900002</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>60</v>
       </c>
@@ -2123,7 +2122,7 @@
         <v>261.06055494399999</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>60</v>
       </c>
@@ -2131,7 +2130,7 @@
         <v>242.615882056</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>61</v>
       </c>
@@ -2139,7 +2138,7 @@
         <v>232.88345161700002</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>61</v>
       </c>
@@ -2147,7 +2146,7 @@
         <v>228.859540885</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>61</v>
       </c>
@@ -2155,7 +2154,7 @@
         <v>228.422382946</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>62</v>
       </c>
@@ -2163,7 +2162,7 @@
         <v>231.76766238600001</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>62</v>
       </c>
@@ -2171,7 +2170,7 @@
         <v>221.321304086</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>62</v>
       </c>
@@ -2179,7 +2178,7 @@
         <v>218.44888661800002</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>63</v>
       </c>
@@ -2187,7 +2186,7 @@
         <v>63.568407706999999</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>63</v>
       </c>
@@ -2195,7 +2194,7 @@
         <v>60.785224855000003</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>63</v>
       </c>
@@ -2203,7 +2202,7 @@
         <v>60.001213186000001</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>64</v>
       </c>
@@ -2211,7 +2210,7 @@
         <v>46.680858495000003</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>64</v>
       </c>
@@ -2219,7 +2218,7 @@
         <v>47.589350416000002</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>64</v>
       </c>
@@ -2227,7 +2226,7 @@
         <v>43.877658973999999</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>65</v>
       </c>
@@ -2235,7 +2234,7 @@
         <v>33.763027303000001</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>65</v>
       </c>
@@ -2243,7 +2242,7 @@
         <v>40.818419261999999</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>65</v>
       </c>
@@ -2251,7 +2250,7 @@
         <v>37.397300585000004</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>66</v>
       </c>
@@ -2259,7 +2258,7 @@
         <v>42.335509600000002</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>66</v>
       </c>
@@ -2267,7 +2266,7 @@
         <v>39.431004342000001</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>66</v>
       </c>
@@ -2275,7 +2274,7 @@
         <v>40.412024854999999</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>67</v>
       </c>
@@ -2283,7 +2282,7 @@
         <v>33.878798012000004</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>67</v>
       </c>
@@ -2291,7 +2290,7 @@
         <v>31.891239553000002</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>67</v>
       </c>
@@ -2299,7 +2298,7 @@
         <v>32.309450416000004</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>68</v>
       </c>
@@ -2307,7 +2306,7 @@
         <v>30.948062259</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>68</v>
       </c>
@@ -2315,7 +2314,7 @@
         <v>29.592786062000002</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>68</v>
       </c>
@@ -2323,7 +2322,7 @@
         <v>30.225424855</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>69</v>
       </c>
@@ -2331,7 +2330,7 @@
         <v>40.164592341000002</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>69</v>
       </c>
@@ -2339,7 +2338,7 @@
         <v>38.421053884999999</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>69</v>
       </c>
@@ -2347,7 +2346,7 @@
         <v>37.558146999000002</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>70</v>
       </c>
@@ -2355,7 +2354,7 @@
         <v>35.340167647999998</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>70</v>
       </c>
@@ -2363,7 +2362,7 @@
         <v>32.698272938000002</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>70</v>
       </c>
@@ -2371,7 +2370,7 @@
         <v>33.790582055999998</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>71</v>
       </c>
@@ -2379,7 +2378,7 @@
         <v>32.989405966</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>71</v>
       </c>
@@ -2387,7 +2386,7 @@
         <v>31.786113841000002</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>71</v>
       </c>
@@ -2395,7 +2394,7 @@
         <v>32.309093885000003</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>72</v>
       </c>
@@ -2403,7 +2402,7 @@
         <v>26.310663542</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>72</v>
       </c>
@@ -2411,7 +2410,7 @@
         <v>30.936653267000001</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>72</v>
       </c>
@@ -2419,7 +2418,7 @@
         <v>29.318766522000001</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>73</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>29.173200008000002</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>73</v>
       </c>
@@ -2435,7 +2434,7 @@
         <v>27.168833659000001</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>73</v>
       </c>
@@ -2443,7 +2442,7 @@
         <v>25.616090221</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>74</v>
       </c>
@@ -2451,7 +2450,7 @@
         <v>43.959355506000001</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>74</v>
       </c>
@@ -2459,7 +2458,7 @@
         <v>40.862883771</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>74</v>
       </c>
@@ -2467,7 +2466,7 @@
         <v>43.467852055999998</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>75</v>
       </c>
@@ -2475,7 +2474,7 @@
         <v>100.268282723</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>75</v>
       </c>
@@ -2483,7 +2482,7 @@
         <v>103.927971572</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>75</v>
       </c>
@@ -2491,7 +2490,7 @@
         <v>102.040802056</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>76</v>
       </c>
@@ -2499,7 +2498,7 @@
         <v>113.969565321</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>76</v>
       </c>
@@ -2507,7 +2506,7 @@
         <v>119.952562965</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>76</v>
       </c>
@@ -2515,7 +2514,7 @@
         <v>117.163370019</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>77</v>
       </c>
@@ -2523,7 +2522,7 @@
         <v>113.65571617500001</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>77</v>
       </c>
@@ -2531,7 +2530,7 @@
         <v>107.13425485500001</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>77</v>
       </c>
@@ -2539,7 +2538,7 @@
         <v>106.568236426</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>78</v>
       </c>
@@ -2547,7 +2546,7 @@
         <v>2.176570822</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>78</v>
       </c>
@@ -2555,7 +2554,7 @@
         <v>2.0724637700000001</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>78</v>
       </c>
@@ -2563,7 +2562,7 @@
         <v>2.1058248850000001</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>79</v>
       </c>
@@ -2571,7 +2570,7 @@
         <v>2.964555265</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>79</v>
       </c>
@@ -2579,7 +2578,7 @@
         <v>2.7691253439999999</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>79</v>
       </c>
@@ -2587,7 +2586,7 @@
         <v>2.833657455</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>80</v>
       </c>
@@ -2595,7 +2594,7 @@
         <v>4.1572023930000004</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>80</v>
       </c>
@@ -2603,7 +2602,7 @@
         <v>4.041177019</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>80</v>
       </c>
@@ -2611,7 +2610,7 @@
         <v>3.688924391</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>81</v>
       </c>
@@ -2619,7 +2618,7 @@
         <v>0.78650738600000003</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>81</v>
       </c>
@@ -2627,7 +2626,7 @@
         <v>0.88343288500000006</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>81</v>
       </c>
@@ -2635,7 +2634,7 @@
         <v>1.0983701450000001</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>82</v>
       </c>
@@ -2643,7 +2642,7 @@
         <v>1.3564985890000001</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>82</v>
       </c>
@@ -2651,7 +2650,7 @@
         <v>1.2427652</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>82</v>
       </c>
@@ -2659,7 +2658,7 @@
         <v>1.302254944</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>83</v>
       </c>
@@ -2667,7 +2666,7 @@
         <v>1.0873176840000001</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>83</v>
       </c>
@@ -2675,7 +2674,7 @@
         <v>0.99884706300000003</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>83</v>
       </c>
@@ -2683,7 +2682,7 @@
         <v>1.022174377</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>84</v>
       </c>
@@ -2691,7 +2690,7 @@
         <v>0.75574385399999999</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>84</v>
       </c>
@@ -2699,7 +2698,7 @@
         <v>0.76572672200000003</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>84</v>
       </c>
@@ -2707,7 +2706,7 @@
         <v>0.80958003499999998</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>85</v>
       </c>
@@ -2715,7 +2714,7 @@
         <v>0.91353428800000003</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>85</v>
       </c>
@@ -2723,7 +2722,7 @@
         <v>0.93563921000000005</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>85</v>
       </c>
@@ -2731,7 +2730,7 @@
         <v>0.91852572200000004</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>86</v>
       </c>
@@ -2739,7 +2738,7 @@
         <v>0.96650460800000004</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>86</v>
       </c>
@@ -2747,7 +2746,7 @@
         <v>0.85277121900000008</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>86</v>
       </c>
@@ -2755,7 +2754,7 @@
         <v>0.89305922199999999</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>87</v>
       </c>
@@ -2763,7 +2762,7 @@
         <v>0.86866231500000002</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>87</v>
       </c>
@@ -2771,7 +2770,7 @@
         <v>0.84207528900000006</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>87</v>
       </c>
@@ -2779,7 +2778,7 @@
         <v>0.86244848900000004</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>88</v>
       </c>
@@ -2787,7 +2786,7 @@
         <v>0.93380562200000006</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>88</v>
       </c>
@@ -2795,7 +2794,7 @@
         <v>0.93986664900000005</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>88</v>
       </c>
@@ -2803,7 +2802,7 @@
         <v>1.036130019</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>89</v>
       </c>
@@ -2811,7 +2810,7 @@
         <v>0.89305922199999999</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>89</v>
       </c>
@@ -2819,7 +2818,7 @@
         <v>0.86759272200000004</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>89</v>
       </c>
@@ -2833,18 +2832,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3071,18 +3070,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{517A7D10-6F5E-4179-A6F2-9FB77FEAB4D7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86CBBAF8-BC64-4CC9-861B-03F9967904D4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86CBBAF8-BC64-4CC9-861B-03F9967904D4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{517A7D10-6F5E-4179-A6F2-9FB77FEAB4D7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>